<commit_message>
modif plan de test
</commit_message>
<xml_diff>
--- a/plan-de-test-P5.xlsx
+++ b/plan-de-test-P5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\phil\FORMATION\OPENCLASSROOM\PARCOURS DEV WEB\PROJET 5 - CONSTRUISEZ UN SITE DE E-COMMERCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\phil\FORMATION\OPENCLASSROOM\PARCOURS DEV WEB\PROJET 5 - CONSTRUISEZ UN SITE DE E-COMMERCE\ORINOCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFD0F5C-1094-41DA-A536-3AAEAB44FA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19901C69-5573-4FB9-91E0-A67F8FB9DEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,7 +918,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modif test et ajout read.md
</commit_message>
<xml_diff>
--- a/plan-de-test-P5.xlsx
+++ b/plan-de-test-P5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\phil\FORMATION\OPENCLASSROOM\PARCOURS DEV WEB\PROJET 5 - CONSTRUISEZ UN SITE DE E-COMMERCE\ORINOCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19901C69-5573-4FB9-91E0-A67F8FB9DEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC330318-61CC-4B8D-8374-A3851132FBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,7 +918,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>